<commit_message>
Removed dead code from edi2odx. Changed Legend key to Annotation
</commit_message>
<xml_diff>
--- a/markers.xlsx
+++ b/markers.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Zoom</t>
   </si>
   <si>
-    <t xml:space="preserve">Legend</t>
+    <t xml:space="preserve">Annotation</t>
   </si>
   <si>
     <t xml:space="preserve">Legend : Green=LW / Blue=MW</t>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added annotation tab. Donesn't process \n from excel:-(
</commit_message>
<xml_diff>
--- a/markers.xlsx
+++ b/markers.xlsx
@@ -9,7 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="Points" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Settings" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Annotations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Settings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Instructions" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -71,10 +73,62 @@
     <t xml:space="preserve">Moldova Grigoriopol 1550 kHz</t>
   </si>
   <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
     <t xml:space="preserve">Title</t>
   </si>
   <si>
-    <t xml:space="preserve">Map of the stations received in Long- and Medium-waves</t>
+    <t xml:space="preserve">Map of the stations received in Long- and Medium-waves from Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TopLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Received on a LW/MW car radio without external antenna on xx.10.2023, yyh UTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TopRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BottomLeft</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Plot: OsmMarker by Ynovo\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Map data: OpenStreetMap</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BottomRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend : Green=Long Waves / Blue=Medium Waves</t>
   </si>
   <si>
     <t xml:space="preserve">MinLon</t>
@@ -96,6 +150,18 @@
   </si>
   <si>
     <t xml:space="preserve">Legend : Green=LW / Blue=MW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/X11_color_names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font size :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float or {'xx-small', 'x-small', 'small', 'medium', 'large', 'x-large', 'xx-large'}</t>
   </si>
 </sst>
 </file>
@@ -105,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -129,16 +195,41 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,8 +266,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -184,12 +279,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -212,13 +315,13 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,7 +342,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
@@ -248,10 +351,10 @@
       <c r="C2" s="2" t="n">
         <v>36.95194</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -390,71 +493,198 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>-10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>-10</v>
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>65</v>
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>24</v>
+      <c r="A6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -466,4 +696,47 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A6:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="https://en.wikipedia.org/wiki/X11_color_names"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
\n processing added in the annotation strings!
</commit_message>
<xml_diff>
--- a/markers.xlsx
+++ b/markers.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">BottomLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend:\nGreen=Long Waves\nBlue=Medium Waves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BottomRight</t>
   </si>
   <si>
     <r>
@@ -125,12 +131,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">BottomRight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legend : Green=Long Waves / Blue=Medium Waves</t>
-  </si>
-  <si>
     <t xml:space="preserve">MinLon</t>
   </si>
   <si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t xml:space="preserve">float or {'xx-small', 'x-small', 'small', 'medium', 'large', 'x-large', 'xx-large'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possibility to use \n in strings to change line</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,32 +568,34 @@
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3"/>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
     </row>
     <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3"/>
@@ -703,10 +708,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A6:B7"/>
+  <dimension ref="A6:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -725,6 +730,11 @@
       </c>
       <c r="B7" s="0" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Markerstyle added. Doc of Excel in Excel, readme updated
</commit_message>
<xml_diff>
--- a/markers.xlsx
+++ b/markers.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -40,18 +40,27 @@
     <t xml:space="preserve">Color</t>
   </si>
   <si>
+    <t xml:space="preserve">MarkerStyle</t>
+  </si>
+  <si>
     <t xml:space="preserve">RX QTH</t>
   </si>
   <si>
     <t xml:space="preserve">red</t>
   </si>
   <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
     <t xml:space="preserve">Algeria Tiapaza 252 kHz</t>
   </si>
   <si>
     <t xml:space="preserve">green</t>
   </si>
   <si>
+    <t xml:space="preserve">o</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hungary Solt 540 kHz</t>
   </si>
   <si>
@@ -79,7 +88,7 @@
     <t xml:space="preserve">Title</t>
   </si>
   <si>
-    <t xml:space="preserve">Map of the stations received in Long- and Medium-waves from Greece</t>
+    <t xml:space="preserve">Some stations received in Long- and Medium-waves from Pylos-Greece</t>
   </si>
   <si>
     <t xml:space="preserve">medium</t>
@@ -91,7 +100,7 @@
     <t xml:space="preserve">TopLeft</t>
   </si>
   <si>
-    <t xml:space="preserve">Received on a LW/MW car radio without external antenna on 4.10.2023, 20h UTC</t>
+    <t xml:space="preserve">Received on a standard LW/MW car radio without external antenna on 4.10.2023, 20h UTC</t>
   </si>
   <si>
     <t xml:space="preserve">X-small</t>
@@ -112,7 +121,7 @@
     <t xml:space="preserve">BottomRight</t>
   </si>
   <si>
-    <t xml:space="preserve">Plot: OsmMarker by Ynovo\nMap data: OpenStreetMap</t>
+    <t xml:space="preserve">Plot: OsmMarker by Ynovo\nMap data: OpenStreetMap\nTransmitter locations: Wikipedia&amp;fmscan.org</t>
   </si>
   <si>
     <t xml:space="preserve">MinLon</t>
@@ -130,19 +139,121 @@
     <t xml:space="preserve">Zoom</t>
   </si>
   <si>
+    <t xml:space="preserve">Script usage described in README.md file</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://github.com/HB9DTX/OsmMarkers/blob/master/README.md</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings to be adjusted in this excel file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not used. For documentation purposes only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive values : East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive values : North</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marker size in points</t>
+  </si>
+  <si>
     <t xml:space="preserve">Colors</t>
   </si>
   <si>
     <t xml:space="preserve">https://en.wikipedia.org/wiki/X11_color_names</t>
   </si>
   <si>
-    <t xml:space="preserve">Font size :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float or {'xx-small', 'x-small', 'small', 'medium', 'large', 'x-large', 'xx-large'}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possibility to use \n in strings for new line</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://matplotlib.org/stable/api/markers_api.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Annotation tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used by python code. Do not change !</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Annotation text. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Possibility to use \n in strings for new line in the same comment</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Font Size : float or {'xx-small', 'x-small', 'small', 'medium', 'large', 'x-large', 'xx-large'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">«Left» Border of the map. Positive values : East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">«Right» border of the map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">«Lower» border of the map. Positive values North</t>
+  </si>
+  <si>
+    <t xml:space="preserve">«Upper» border of the map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenStreetmap zoom factor. Gives the amount of details. To be tested by trial and error</t>
   </si>
 </sst>
 </file>
@@ -152,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -188,11 +299,31 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -243,7 +374,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -268,6 +399,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,10 +424,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,10 +452,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>21.69514</v>
@@ -328,12 +470,15 @@
         <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>2.480639</v>
@@ -345,12 +490,15 @@
         <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>19.031567</v>
@@ -362,12 +510,15 @@
         <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>31.130333</v>
@@ -379,12 +530,15 @@
         <v>20</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>60.612778</v>
@@ -396,12 +550,15 @@
         <v>20</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>23.807611</v>
@@ -413,12 +570,15 @@
         <v>20</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>35.590833</v>
@@ -430,12 +590,15 @@
         <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>29.436667</v>
@@ -447,7 +610,10 @@
         <v>20</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -469,7 +635,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -496,70 +662,70 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,7 +772,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -616,7 +782,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="n">
         <v>-10</v>
@@ -624,7 +790,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>65</v>
@@ -632,7 +798,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>20</v>
@@ -640,7 +806,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>60</v>
@@ -648,7 +814,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>4</v>
@@ -670,38 +836,179 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A6:B10"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>38</v>
+      <c r="A7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="https://en.wikipedia.org/wiki/X11_color_names"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://github.com/HB9DTX/OsmMarkers/blob/master/README.md"/>
+    <hyperlink ref="B12" r:id="rId2" display="https://en.wikipedia.org/wiki/X11_color_names"/>
+    <hyperlink ref="B13" r:id="rId3" display="https://matplotlib.org/stable/api/markers_api.html"/>
+    <hyperlink ref="B19" r:id="rId4" display="https://en.wikipedia.org/wiki/X11_color_names"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
.lower() added to color parameter to cope with Excel/Libreoffice Calc automatic first uppercase Colors updated
</commit_message>
<xml_diff>
--- a/markers.xlsx
+++ b/markers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Points" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -64,140 +64,28 @@
     <t xml:space="preserve">Hungary Solt 540 kHz</t>
   </si>
   <si>
-    <t xml:space="preserve">blue</t>
+    <t xml:space="preserve">chocolate</t>
   </si>
   <si>
     <t xml:space="preserve">Egypt Santah 865 kHz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romania Yekaterinburg 909kHz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romania Cluj-Napoca 1150 kHz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saudi Arabia Duba (tbk)1520 kHz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moldova Grigoriopol 1550 kHz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some stations received in Long- and Medium-waves from Pylos-Greece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TopLeft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Received on a standard LW/MW car radio without external antenna on 4.10.2023, 20h UTC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X-small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TopRight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BottomLeft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legend:\nGreen=Long Waves\nBlue=Medium Waves\nRed=Receiver location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BottomRight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plot: OsmMarker by Ynovo\nMap data: OpenStreetMap\nTransmitter locations: Wikipedia&amp;fmscan.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MinLon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MinLat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Script usage described in README.md file</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/HB9DTX/OsmMarkers/blob/master/README.md</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">Romania </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Settings to be adjusted in this excel file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Points tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not used. For documentation purposes only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive values : East</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive values : North</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marker size in points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://en.wikipedia.org/wiki/X11_color_names</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://matplotlib.org/stable/api/markers_api.html</t>
+      <t xml:space="preserve">Cluj-Napoca</t>
     </r>
     <r>
       <rPr>
@@ -206,33 +94,119 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> 909kHz</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Romania Cluj-Napoca 1150 kHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saudi Arabia Duba (tbk)1520 kHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moldova Grigoriopol 1550 kHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some stations received in Long- and Medium-waves from Pylos-Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TopLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Received on a standard LW/MW car radio without external antenna on 4.10.2023, 20h UTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TopRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BottomLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green=Longwaves transmitter\nBrown=Mediumwave transmitters\nRed=Receiver location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BottomRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot: OsmMarker by Ynovo\nMap data: OpenStreetMap\nTransmitter locations: Wikipedia&amp;fmscan.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinLon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxLon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinLat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxLat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Script usage described in README.md file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/HB9DTX/OsmMarkers/blob/master/README.md </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings to be adjusted in this excel file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not used. For documentation purposes only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive values : East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive values : North</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marker size in points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://matplotlib.org/stable/gallery/color/named_colors.html#css-colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://matplotlib.org/stable/api/markers_api.html </t>
+  </si>
+  <si>
     <t xml:space="preserve">Annotation tab</t>
   </si>
   <si>
     <t xml:space="preserve">Used by python code. Do not change !</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Annotation text. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Possibility to use \n in strings for new line in the same comment</t>
-    </r>
+    <t xml:space="preserve">Annotation text. Possibility to use \n in strings for new line in the same comment</t>
   </si>
   <si>
     <t xml:space="preserve">Font Size : float or {'xx-small', 'x-small', 'small', 'medium', 'large', 'x-large', 'xx-large'}</t>
@@ -294,6 +268,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
@@ -319,11 +298,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -391,10 +365,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -404,6 +374,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,10 +401,10 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.16"/>
@@ -467,7 +441,7 @@
         <v>36.95194</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -487,7 +461,7 @@
         <v>36.56615</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>10</v>
@@ -507,7 +481,7 @@
         <v>46.834308</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>13</v>
@@ -527,7 +501,7 @@
         <v>30.735167</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>13</v>
@@ -541,13 +515,13 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>60.612778</v>
+        <v>23.807611</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>56.835556</v>
+        <v>46.867139</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>13</v>
@@ -567,7 +541,7 @@
         <v>46.867139</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>13</v>
@@ -587,7 +561,7 @@
         <v>27.444444</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>13</v>
@@ -607,7 +581,7 @@
         <v>47.280278</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>13</v>
@@ -634,11 +608,11 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.02"/>
@@ -685,47 +659,47 @@
         <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,18 +745,18 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="n">
         <v>-10</v>
@@ -790,31 +764,31 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>4</v>
@@ -839,19 +813,19 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,7 +836,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +844,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,15 +876,15 @@
         <v>3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,12 +892,12 @@
         <v>5</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,7 +913,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,68 +921,66 @@
         <v>3</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://github.com/HB9DTX/OsmMarkers/blob/master/README.md"/>
-    <hyperlink ref="B12" r:id="rId2" display="https://en.wikipedia.org/wiki/X11_color_names"/>
-    <hyperlink ref="B13" r:id="rId3" display="https://matplotlib.org/stable/api/markers_api.html"/>
-    <hyperlink ref="B19" r:id="rId4" display="https://en.wikipedia.org/wiki/X11_color_names"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://github.com/HB9DTX/OsmMarkers/blob/master/README.md "/>
+    <hyperlink ref="B13" r:id="rId2" display="https://matplotlib.org/stable/api/markers_api.html "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>